<commit_message>
Updated: Test Cases and Requirements list
</commit_message>
<xml_diff>
--- a/src/vision/Test_Cases.xlsx
+++ b/src/vision/Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\bhoomi-vision\src\vision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E20A09-2579-4FC8-8A5B-B14379F77F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A29E23C-CF69-48AD-825C-1253C2FA5D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{319483C9-5B55-4C78-96B6-E34C7372EE60}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{319483C9-5B55-4C78-96B6-E34C7372EE60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Test Scenarios </t>
   </si>
@@ -53,15 +53,9 @@
     <t>Image input with different format</t>
   </si>
   <si>
-    <t>Video input with different format</t>
-  </si>
-  <si>
     <t>Correct input to API</t>
   </si>
   <si>
-    <t>Checking frame detection</t>
-  </si>
-  <si>
     <t>Input Frame with no plant</t>
   </si>
   <si>
@@ -74,13 +68,44 @@
     <t xml:space="preserve">Input Frame with zoomed in plant </t>
   </si>
   <si>
-    <t>Multiple Image upload</t>
-  </si>
-  <si>
-    <t>Comparison with actual size of plants</t>
-  </si>
-  <si>
-    <t>Compare plant height list with actual list</t>
+    <t>Image stream input with frames in a folder</t>
+  </si>
+  <si>
+    <t>Coordinates associated with each frame in the form (lat, long, height)</t>
+  </si>
+  <si>
+    <t>Coordintes not present with a frame</t>
+  </si>
+  <si>
+    <t>Incomplete coordinates of a frame</t>
+  </si>
+  <si>
+    <t>Deduplication</t>
+  </si>
+  <si>
+    <t>Repeated frame with complete overlap</t>
+  </si>
+  <si>
+    <t>Partial overlap between two frames</t>
+  </si>
+  <si>
+    <t>No overlap between frames</t>
+  </si>
+  <si>
+    <t>Frame detection</t>
+  </si>
+  <si>
+    <t>ROI mapping</t>
+  </si>
+  <si>
+    <t>Bounding box with four points defined for each type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API Output </t>
+  </si>
+  <si>
+    <t>Capturing parameters {droneID, CameraID, Timestamp, LocationID, RegionID, 
+PlantGrowth, PlantID}</t>
   </si>
 </sst>
 </file>
@@ -468,11 +493,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DF9CCC3-CAF5-4690-AC41-1F89AC3A885C}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -502,7 +525,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -514,27 +537,25 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -543,16 +564,18 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -561,22 +584,80 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>